<commit_message>
Attēli un papilddati sugu rezultātiem
</commit_message>
<xml_diff>
--- a/Papilddati/EGV_putniem.xlsx
+++ b/Papilddati/EGV_putniem.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrisavotins/Documents/projekti/LVAFA_SDMs/Darbam/PutnuSDMs_gramata/Papilddati/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrisavotins/Documents/projekti/LVAFA_SDMs/Darbam/LVAFA_SDMs/Rastri_100m/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AADEA5E-F1BA-BF43-BA50-1A721FC86544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5180BE23-6A68-4746-A0D4-7D7E1F98EC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36000" yWindow="620" windowWidth="34560" windowHeight="22960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4123,10 +4123,10 @@
   <dimension ref="A1:DQ339"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="BD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BG2" sqref="BG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4655,9 +4655,6 @@
       <c r="BF2">
         <v>1</v>
       </c>
-      <c r="BG2">
-        <v>1</v>
-      </c>
       <c r="BI2">
         <v>1</v>
       </c>
@@ -4853,9 +4850,6 @@
       <c r="BF5">
         <v>1</v>
       </c>
-      <c r="BG5">
-        <v>1</v>
-      </c>
       <c r="BI5">
         <v>1</v>
       </c>
@@ -4898,9 +4892,6 @@
         <v>1</v>
       </c>
       <c r="BE6">
-        <v>1</v>
-      </c>
-      <c r="BG6">
         <v>1</v>
       </c>
       <c r="BI6">

</xml_diff>